<commit_message>
edit sim cluster code
</commit_message>
<xml_diff>
--- a/Documentation/Simulation computation times.xlsx
+++ b/Documentation/Simulation computation times.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -131,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -146,6 +149,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,17 +890,17 @@
         <v>0.52222222222222225</v>
       </c>
       <c r="M13" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N13" s="4">
         <f>M13*H13</f>
-        <v>3.8888888888889639E-2</v>
+        <v>4.3750000000000844E-2</v>
       </c>
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>42579</v>
+        <v>42578</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -932,17 +936,17 @@
         <v>0.52708333333333335</v>
       </c>
       <c r="M14" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" ref="N14:N16" si="2">M14*H14</f>
-        <v>3.8888888888888751E-2</v>
+        <v>4.3749999999999845E-2</v>
       </c>
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>42580</v>
+        <v>42578</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -978,17 +982,17 @@
         <v>0.55902777777777779</v>
       </c>
       <c r="M15" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="2"/>
-        <v>0.25555555555555554</v>
+        <v>0.28749999999999998</v>
       </c>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>42581</v>
+        <v>42578</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
@@ -1024,70 +1028,122 @@
         <v>0.59375</v>
       </c>
       <c r="M16" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" si="2"/>
-        <v>0.27777777777777768</v>
+        <v>0.31249999999999989</v>
       </c>
       <c r="O16" s="4">
-        <v>0.66666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="P16" s="4">
-        <f>SUM(N13:N16)</f>
-        <v>0.6111111111111116</v>
-      </c>
-      <c r="Q16" s="4">
+        <f>SUM(N13:N16) *4</f>
+        <v>2.7500000000000022</v>
+      </c>
+      <c r="Q16" s="8">
         <f>O16+P16</f>
-        <v>1.2777777777777781</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
+        <v>3.3750000000000022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>42578</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>1200</v>
+      </c>
+      <c r="F17">
+        <v>5000</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17" si="3">E17*F17</f>
+        <v>6000000</v>
+      </c>
+      <c r="H17" s="5">
+        <f>L17-K17</f>
+        <v>1.8749999999999933E-2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="M17" s="7">
+        <v>9</v>
+      </c>
+      <c r="N17" s="4">
+        <f>M17*H17</f>
+        <v>0.1687499999999994</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="P17" s="4">
+        <f>H17</f>
+        <v>1.8749999999999933E-2</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>O17+P17</f>
+        <v>0.6854166666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new sim results done so added times to documentation
</commit_message>
<xml_diff>
--- a/Documentation/Simulation computation times.xlsx
+++ b/Documentation/Simulation computation times.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -89,13 +89,13 @@
     <t>projected end time</t>
   </si>
   <si>
-    <t>increase replicates</t>
-  </si>
-  <si>
     <t>Projected end time for total</t>
   </si>
   <si>
     <t>projected start time</t>
+  </si>
+  <si>
+    <t>time per calculation step</t>
   </si>
 </sst>
 </file>
@@ -103,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -149,7 +149,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,7 +438,7 @@
     <col min="7" max="7" width="25.5" customWidth="1"/>
     <col min="8" max="9" width="43.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="25" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" style="7" customWidth="1"/>
     <col min="14" max="15" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -480,16 +480,16 @@
         <v>15</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N1" t="s">
         <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
         <v>5000</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17" si="3">E17*F17</f>
+        <f t="shared" ref="G17:G25" si="3">E17*F17</f>
         <v>6000000</v>
       </c>
       <c r="H17" s="5">
@@ -1102,31 +1102,287 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I18" s="6"/>
+      <c r="A18" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>1200</v>
+      </c>
+      <c r="F18">
+        <v>5000</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H18"/>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18"/>
+      <c r="M18"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I19" s="6"/>
+      <c r="A19" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <v>1200</v>
+      </c>
+      <c r="F19">
+        <v>5000</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19"/>
+      <c r="M19"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I20" s="6"/>
+      <c r="A20" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>1200</v>
+      </c>
+      <c r="F20">
+        <v>5000</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20"/>
+      <c r="M20"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I21" s="6"/>
+      <c r="A21" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>1200</v>
+      </c>
+      <c r="F21">
+        <v>5000</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21"/>
+      <c r="M21"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I22" s="6"/>
+      <c r="A22" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>1200</v>
+      </c>
+      <c r="F22">
+        <v>5000</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H22" s="5">
+        <f>L22-K22</f>
+        <v>0.10486111111111118</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22" s="4">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="L22" s="4">
+        <f>K23</f>
+        <v>0.74444444444444446</v>
+      </c>
+      <c r="M22"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I23" s="6"/>
+      <c r="A23" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>28</v>
+      </c>
+      <c r="E23">
+        <v>1200</v>
+      </c>
+      <c r="F23">
+        <v>5000</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ref="H23:H25" si="4">L23-K23</f>
+        <v>0.11597222222222214</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23"/>
+      <c r="K23" s="4">
+        <v>0.74444444444444446</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" ref="L23:L24" si="5">K24</f>
+        <v>0.86041666666666661</v>
+      </c>
+      <c r="M23"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I24" s="6"/>
+      <c r="A24" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>1200</v>
+      </c>
+      <c r="F24">
+        <v>5000</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H24" s="6">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24"/>
+      <c r="K24" s="4">
+        <v>0.86041666666666661</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="5"/>
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="M24"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I25" s="6"/>
+      <c r="A25" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>1200</v>
+      </c>
+      <c r="F25">
+        <v>5000</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>6000000</v>
+      </c>
+      <c r="H25" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25"/>
+      <c r="K25" s="4">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="M25"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I26" s="6"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="M26"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I27" s="6"/>

</xml_diff>

<commit_message>
fix large file upload error
</commit_message>
<xml_diff>
--- a/Documentation/Simulation computation times.xlsx
+++ b/Documentation/Simulation computation times.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -430,7 +430,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1125,7 @@
         <v>6000000</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" ref="H18:H21" si="4">L18-K18</f>
+        <f t="shared" ref="H18:H19" si="4">L18-K18</f>
         <v>0.19513888888888886</v>
       </c>
       <c r="I18">
@@ -1322,7 +1322,7 @@
         <v>6000000</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" ref="H23:H25" si="6">L23-K23</f>
+        <f t="shared" ref="H23" si="6">L23-K23</f>
         <v>0.11597222222222214</v>
       </c>
       <c r="I23">
@@ -1416,19 +1416,132 @@
       <c r="M25"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H26"/>
-      <c r="I26"/>
+      <c r="A26" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>1200</v>
+      </c>
+      <c r="F26">
+        <v>10000</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="8">E26*F26</f>
+        <v>12000000</v>
+      </c>
+      <c r="H26" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
       <c r="J26"/>
       <c r="M26"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I27" s="6"/>
+      <c r="A27" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>28</v>
+      </c>
+      <c r="E27">
+        <v>1200</v>
+      </c>
+      <c r="F27">
+        <v>10000</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="8"/>
+        <v>12000000</v>
+      </c>
+      <c r="H27" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27"/>
+      <c r="M27"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I28" s="6"/>
+      <c r="A28" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>29</v>
+      </c>
+      <c r="E28">
+        <v>1200</v>
+      </c>
+      <c r="F28">
+        <v>10000</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="8"/>
+        <v>12000000</v>
+      </c>
+      <c r="H28" s="6">
+        <v>25.2</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28"/>
+      <c r="M28"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I29" s="6"/>
+      <c r="A29" s="1">
+        <v>42580</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>31</v>
+      </c>
+      <c r="E29">
+        <v>1200</v>
+      </c>
+      <c r="F29">
+        <v>10000</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="8"/>
+        <v>12000000</v>
+      </c>
+      <c r="H29" s="6">
+        <v>25.2</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29"/>
+      <c r="M29"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I30" s="6"/>

</xml_diff>

<commit_message>
trying new c functions
</commit_message>
<xml_diff>
--- a/Documentation/Simulation computation times.xlsx
+++ b/Documentation/Simulation computation times.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1435,7 @@
         <v>10000</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26:G30" si="8">E26*F26</f>
+        <f t="shared" ref="G26:G29" si="8">E26*F26</f>
         <v>12000000</v>
       </c>
       <c r="H26" s="6">
@@ -1664,10 +1664,124 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I34" s="6"/>
+      <c r="A34" s="1">
+        <v>42600</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34">
+        <v>1254</v>
+      </c>
+      <c r="F34">
+        <v>5000</v>
+      </c>
+      <c r="G34">
+        <f>F34*E34</f>
+        <v>6270000</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="I34" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I35" s="6"/>
+      <c r="A35" s="1">
+        <v>42600</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>28</v>
+      </c>
+      <c r="E35">
+        <v>1254</v>
+      </c>
+      <c r="F35">
+        <v>5000</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35:G37" si="10">F35*E35</f>
+        <v>6270000</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>42600</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>29</v>
+      </c>
+      <c r="E36">
+        <v>1254</v>
+      </c>
+      <c r="F36">
+        <v>5000</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="10"/>
+        <v>6270000</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>42600</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>31</v>
+      </c>
+      <c r="E37">
+        <v>1254</v>
+      </c>
+      <c r="F37">
+        <v>5000</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="10"/>
+        <v>6270000</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="I37" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
how long to run?
</commit_message>
<xml_diff>
--- a/Documentation/Simulation computation times.xlsx
+++ b/Documentation/Simulation computation times.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>time per calculation step</t>
+  </si>
+  <si>
+    <t>CHPC</t>
+  </si>
+  <si>
+    <t>Sim+analysis</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1923,7 +1929,7 @@
         <v>50000</v>
       </c>
       <c r="G42">
-        <f t="shared" ref="G42" si="12">F42*E42</f>
+        <f t="shared" ref="G42:G43" si="12">F42*E42</f>
         <v>62700000</v>
       </c>
       <c r="H42" s="2">
@@ -1931,6 +1937,66 @@
       </c>
       <c r="I42" s="6">
         <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42615</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43">
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>1254</v>
+      </c>
+      <c r="F43">
+        <v>10000</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="12"/>
+        <v>12540000</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>42615</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44">
+        <v>31</v>
+      </c>
+      <c r="E44">
+        <v>1254</v>
+      </c>
+      <c r="F44">
+        <v>30000</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44" si="13">F44*E44</f>
+        <v>37620000</v>
+      </c>
+      <c r="H44" s="2">
+        <v>2</v>
+      </c>
+      <c r="I44" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>